<commit_message>
update i3 excel data
</commit_message>
<xml_diff>
--- a/insights/3/solution_approaches.xlsx
+++ b/insights/3/solution_approaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\insights\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B969AF9F-02D5-439B-9501-61C33DEF91BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852052ED-BED5-4813-A9F9-822BFAF68A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>task_name</t>
   </si>
   <si>
-    <t>first_begin_ts</t>
-  </si>
-  <si>
     <t>consecutive_submission_count</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>shoes</t>
+  </si>
+  <si>
+    <t>last_submission_ts</t>
   </si>
 </sst>
 </file>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" activeCellId="1" sqref="D87 G2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,13 +927,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4">
         <v>43683.213429872689</v>
@@ -962,16 +962,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
-        <v>43683.232858078707</v>
+        <v>43683.237084907407</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>1.9428206018518517E-2</v>
+        <v>5.0965393518518521E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4">
         <v>43683.243435949073</v>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>1.0577881944444445E-2</v>
+        <v>2.3655034722222218E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4">
         <v>43683.254285509262</v>
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>1.0849548611111112E-2</v>
+        <v>6.3510416666666672E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="4">
         <v>43683.274482152781</v>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>2.0196655092592594E-2</v>
+        <v>1.0849548611111112E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4">
         <v>43683.304326840276</v>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>2.9844687499999998E-2</v>
+        <v>2.0196655092592594E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,16 +1062,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="4">
-        <v>43683.309803240743</v>
+        <v>43683.408746365742</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
       </c>
       <c r="F8" s="2">
-        <v>5.4764004629629624E-3</v>
+        <v>2.9844687499999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,10 +1082,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4">
-        <v>43683.252460208336</v>
+        <v>43683.253745520837</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -1100,16 +1100,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>43683.275868101853</v>
+        <v>43683.283905393517</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
       </c>
       <c r="F10" s="2">
-        <v>2.3407893518518519E-2</v>
+        <v>4.5412187499999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,16 +1120,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4">
-        <v>43683.297269722221</v>
+        <v>43683.311759560187</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
       </c>
       <c r="F11" s="2">
-        <v>2.1401620370370369E-2</v>
+        <v>3.0159884259259261E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1140,16 +1140,16 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="4">
-        <v>43683.323255740739</v>
+        <v>43683.333764062503</v>
       </c>
       <c r="E12" s="1">
         <v>7</v>
       </c>
       <c r="F12" s="2">
-        <v>2.598603009259259E-2</v>
+        <v>2.7854155092592592E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="4">
         <v>43683.361909803243</v>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>3.8654062500000003E-2</v>
+        <v>2.2004502314814819E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1180,16 +1180,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4">
-        <v>43683.372826782404</v>
+        <v>43683.373733564818</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
       <c r="F14" s="2">
-        <v>1.0916979166666667E-2</v>
+        <v>2.8145752314814813E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1200,16 +1200,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="4">
-        <v>43683.41021908565</v>
+        <v>43683.415224687502</v>
       </c>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="2">
-        <v>3.7392303240740742E-2</v>
+        <v>1.1823749999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="4">
         <v>43683.219143668983</v>
@@ -1238,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4">
         <v>43683.221766493058</v>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>2.6228240740740743E-3</v>
+        <v>1.0810335648148149E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,16 +1258,16 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4">
-        <v>43683.290256898152</v>
+        <v>43683.298311250001</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="2">
-        <v>6.8490405092592591E-2</v>
+        <v>2.6228240740740743E-3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,16 +1278,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="4">
-        <v>43683.313094363424</v>
+        <v>43683.313890173609</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="2">
-        <v>2.2837465277777778E-2</v>
+        <v>7.6544756944444445E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,16 +1298,16 @@
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="4">
-        <v>43683.325297523152</v>
+        <v>43683.326026331022</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20" s="2">
-        <v>1.2203159722222223E-2</v>
+        <v>1.5578923611111113E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,16 +1318,16 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" s="4">
-        <v>43683.33167255787</v>
+        <v>43683.344978749999</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
       </c>
       <c r="F21" s="2">
-        <v>6.3750231481481479E-3</v>
+        <v>1.2136157407407408E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,16 +1338,16 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="4">
-        <v>43683.357151481483</v>
+        <v>43683.370741956016</v>
       </c>
       <c r="E22" s="1">
         <v>5</v>
       </c>
       <c r="F22" s="2">
-        <v>2.547892361111111E-2</v>
+        <v>1.8952418981481482E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,16 +1358,16 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="4">
-        <v>43683.396079224534</v>
+        <v>43683.407057719909</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
       </c>
       <c r="F23" s="2">
-        <v>3.8927754629629628E-2</v>
+        <v>2.5763206018518517E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,10 +1378,10 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="4">
-        <v>43683.21888591435</v>
+        <v>43683.268858460651</v>
       </c>
       <c r="E24" s="1">
         <v>8</v>
@@ -1396,16 +1396,16 @@
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="4">
-        <v>43683.274139942128</v>
+        <v>43683.281520682867</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
       </c>
       <c r="F25" s="2">
-        <v>5.5254027777777777E-2</v>
+        <v>6.0525127314814818E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,16 +1416,16 @@
         <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="4">
-        <v>43683.292708935187</v>
+        <v>43683.399083298609</v>
       </c>
       <c r="E26" s="1">
         <v>42</v>
       </c>
       <c r="F26" s="2">
-        <v>1.8568993055555556E-2</v>
+        <v>1.2662222222222221E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="4">
         <v>43683.223088749997</v>
@@ -1454,16 +1454,16 @@
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="4">
-        <v>43683.239143159721</v>
+        <v>43683.252301562497</v>
       </c>
       <c r="E28" s="1">
         <v>6</v>
       </c>
       <c r="F28" s="2">
-        <v>1.6054409722222222E-2</v>
+        <v>1.4755416666666667E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" s="4">
         <v>43683.253007118059</v>
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="2">
-        <v>1.3863958333333331E-2</v>
+        <v>2.9212812500000004E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="4">
         <v>43683.254344641202</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="2">
-        <v>1.3375231481481482E-3</v>
+        <v>7.0555555555555562E-4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4">
         <v>43683.255862118058</v>
@@ -1523,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2">
-        <v>1.517465277777778E-3</v>
+        <v>1.3375231481481482E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>15</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="4">
-        <v>43683.257885752311</v>
+        <v>43683.272365092591</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
       </c>
       <c r="F32" s="2">
-        <v>2.0236342592592593E-3</v>
+        <v>1.517465277777778E-3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,16 +1554,16 @@
         <v>15</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="4">
-        <v>43683.29098888889</v>
+        <v>43683.365185810188</v>
       </c>
       <c r="E33" s="1">
         <v>37</v>
       </c>
       <c r="F33" s="2">
-        <v>3.3103136574074078E-2</v>
+        <v>1.650297453703704E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1574,16 +1574,16 @@
         <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="4">
-        <v>43683.377286365743</v>
+        <v>43683.415339502317</v>
       </c>
       <c r="E34" s="1">
         <v>17</v>
       </c>
       <c r="F34" s="2">
-        <v>8.6297476851851851E-2</v>
+        <v>9.2820717592592597E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,10 +1594,10 @@
         <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="4">
-        <v>43683.22387991898</v>
+        <v>43683.227955046299</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
@@ -1612,16 +1612,16 @@
         <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" s="4">
-        <v>43683.273924988425</v>
+        <v>43683.292882870373</v>
       </c>
       <c r="E36" s="1">
         <v>9</v>
       </c>
       <c r="F36" s="2">
-        <v>5.004505787037037E-2</v>
+        <v>1.9621712962962962E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,16 +1632,16 @@
         <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="4">
-        <v>43683.304149768519</v>
+        <v>43683.339412314817</v>
       </c>
       <c r="E37" s="1">
         <v>8</v>
       </c>
       <c r="F37" s="2">
-        <v>3.0224780092592593E-2</v>
+        <v>6.4927824074074061E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,16 +1652,16 @@
         <v>16</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="4">
-        <v>43683.342820219907</v>
+        <v>43683.343542303242</v>
       </c>
       <c r="E38" s="1">
         <v>2</v>
       </c>
       <c r="F38" s="2">
-        <v>3.8670451388888895E-2</v>
+        <v>4.652944444444445E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,16 +1672,16 @@
         <v>16</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" s="4">
-        <v>43683.353793796297</v>
+        <v>43683.41037986111</v>
       </c>
       <c r="E39" s="1">
         <v>40</v>
       </c>
       <c r="F39" s="2">
-        <v>1.097357638888889E-2</v>
+        <v>4.1299884259259258E-3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="4">
         <v>43683.221433668979</v>
@@ -1710,7 +1710,7 @@
         <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" s="4">
         <v>43683.226922928239</v>
@@ -1719,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="2">
-        <v>5.4892592592592597E-3</v>
+        <v>1.3100335648148149E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42" s="4">
         <v>43683.237672835647</v>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2">
-        <v>1.0749907407407408E-2</v>
+        <v>5.4892592592592597E-3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="4">
         <v>43683.252146886574</v>
@@ -1759,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="2">
-        <v>1.4474050925925923E-2</v>
+        <v>1.0749907407407408E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,16 +1770,16 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44" s="4">
-        <v>43683.261672708337</v>
+        <v>43683.275422025465</v>
       </c>
       <c r="E44" s="1">
         <v>3</v>
       </c>
       <c r="F44" s="2">
-        <v>9.5258333333333323E-3</v>
+        <v>1.4474050925925923E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1790,16 +1790,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45" s="4">
-        <v>43683.281766631946</v>
+        <v>43683.290033275465</v>
       </c>
       <c r="E45" s="1">
         <v>2</v>
       </c>
       <c r="F45" s="2">
-        <v>2.0093923611111109E-2</v>
+        <v>2.327513888888889E-2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1810,16 +1810,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="4">
-        <v>43683.326016458333</v>
+        <v>43683.357367453704</v>
       </c>
       <c r="E46" s="1">
         <v>6</v>
       </c>
       <c r="F46" s="2">
-        <v>4.4249814814814818E-2</v>
+        <v>1.4611249999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,16 +1830,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="4">
-        <v>43683.383226319442</v>
+        <v>43683.385263773147</v>
       </c>
       <c r="E47" s="1">
         <v>3</v>
       </c>
       <c r="F47" s="2">
-        <v>5.7209861111111114E-2</v>
+        <v>6.7334178240740741E-2</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1850,10 +1850,10 @@
         <v>38</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48" s="4">
-        <v>43683.229829027776</v>
+        <v>43683.27984841435</v>
       </c>
       <c r="E48" s="1">
         <v>8</v>
@@ -1868,16 +1868,16 @@
         <v>38</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49" s="4">
-        <v>43683.294392662036</v>
+        <v>43683.341245474534</v>
       </c>
       <c r="E49" s="1">
         <v>6</v>
       </c>
       <c r="F49" s="2">
-        <v>6.4563634259259262E-2</v>
+        <v>7.1515081018518514E-2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1888,16 +1888,16 @@
         <v>38</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" s="4">
-        <v>43683.364011747683</v>
+        <v>43683.375652870367</v>
       </c>
       <c r="E50" s="1">
         <v>8</v>
       </c>
       <c r="F50" s="2">
-        <v>6.9619085648148157E-2</v>
+        <v>6.1397060185185183E-2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,16 +1908,16 @@
         <v>38</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D51" s="4">
-        <v>43683.397910335647</v>
+        <v>43683.411345995373</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
       </c>
       <c r="F51" s="2">
-        <v>3.389858796296296E-2</v>
+        <v>3.4407395833333333E-2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,10 +1928,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52" s="4">
-        <v>43683.230274097223</v>
+        <v>43683.235839560184</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -1946,16 +1946,16 @@
         <v>50</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" s="4">
-        <v>43683.307140856479</v>
+        <v>43683.315589594909</v>
       </c>
       <c r="E53" s="1">
         <v>5</v>
       </c>
       <c r="F53" s="2">
-        <v>7.686675925925926E-2</v>
+        <v>2.7506226851851851E-2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,16 +1966,16 @@
         <v>50</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54" s="4">
-        <v>43683.339978043979</v>
+        <v>43683.35656871528</v>
       </c>
       <c r="E54" s="1">
         <v>4</v>
       </c>
       <c r="F54" s="2">
-        <v>3.2837187499999997E-2</v>
+        <v>7.975003472222221E-2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,7 +1986,7 @@
         <v>50</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55" s="4">
         <v>43683.358605034722</v>
@@ -1995,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="2">
-        <v>1.8626990740740739E-2</v>
+        <v>4.0979120370370374E-2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2006,16 +2006,16 @@
         <v>50</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56" s="4">
-        <v>43683.379504594908</v>
+        <v>43683.407845324073</v>
       </c>
       <c r="E56" s="1">
         <v>10</v>
       </c>
       <c r="F56" s="2">
-        <v>2.0899560185185184E-2</v>
+        <v>2.0363078703703702E-3</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,10 +2026,10 @@
         <v>54</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" s="4">
-        <v>43683.220228576392</v>
+        <v>43683.263663321763</v>
       </c>
       <c r="E57" s="1">
         <v>11</v>
@@ -2044,16 +2044,16 @@
         <v>54</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="4">
-        <v>43683.270523692132</v>
+        <v>43683.313662719906</v>
       </c>
       <c r="E58" s="1">
         <v>9</v>
       </c>
       <c r="F58" s="2">
-        <v>5.0295115740740741E-2</v>
+        <v>5.5329988425925923E-2</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2064,16 +2064,16 @@
         <v>54</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="4">
-        <v>43683.320077303244</v>
+        <v>43683.330327731484</v>
       </c>
       <c r="E59" s="1">
         <v>4</v>
       </c>
       <c r="F59" s="2">
-        <v>4.9553611111111111E-2</v>
+        <v>4.9999398148148154E-2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,16 +2084,16 @@
         <v>54</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D60" s="4">
-        <v>43683.339945358799</v>
+        <v>43683.350137650465</v>
       </c>
       <c r="E60" s="1">
         <v>10</v>
       </c>
       <c r="F60" s="2">
-        <v>1.9868055555555555E-2</v>
+        <v>1.6665011574074073E-2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>54</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D61" s="4">
         <v>43683.362130925925</v>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="2">
-        <v>2.218556712962963E-2</v>
+        <v>1.9809918981481479E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,16 +2124,16 @@
         <v>54</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D62" s="4">
-        <v>43683.389551631946</v>
+        <v>43683.41025577546</v>
       </c>
       <c r="E62" s="1">
         <v>4</v>
       </c>
       <c r="F62" s="2">
-        <v>2.7420717592592594E-2</v>
+        <v>1.1993275462962963E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,10 +2144,10 @@
         <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D63" s="4">
-        <v>43683.23843986111</v>
+        <v>43683.306910381943</v>
       </c>
       <c r="E63" s="1">
         <v>10</v>
@@ -2162,16 +2162,16 @@
         <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D64" s="4">
-        <v>43683.318867592592</v>
+        <v>43683.329442557872</v>
       </c>
       <c r="E64" s="1">
         <v>5</v>
       </c>
       <c r="F64" s="2">
-        <v>8.0427731481481482E-2</v>
+        <v>9.8577048611111107E-2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2182,16 +2182,16 @@
         <v>84</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D65" s="4">
-        <v>43683.351383564812</v>
+        <v>43683.354216655091</v>
       </c>
       <c r="E65" s="1">
         <v>3</v>
       </c>
       <c r="F65" s="2">
-        <v>3.2515972222222224E-2</v>
+        <v>2.253216435185185E-2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,16 +2202,16 @@
         <v>84</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="4">
-        <v>43683.371336261574</v>
+        <v>43683.382646944447</v>
       </c>
       <c r="E66" s="1">
         <v>2</v>
       </c>
       <c r="F66" s="2">
-        <v>1.9952708333333333E-2</v>
+        <v>2.4774097222222222E-2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,16 +2222,16 @@
         <v>84</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D67" s="4">
-        <v>43683.39578392361</v>
+        <v>43683.413395000003</v>
       </c>
       <c r="E67" s="1">
         <v>15</v>
       </c>
       <c r="F67" s="2">
-        <v>2.4447662037037035E-2</v>
+        <v>2.8430289351851851E-2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,10 +2242,10 @@
         <v>98</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68" s="4">
-        <v>43683.243932974539</v>
+        <v>43683.2666828125</v>
       </c>
       <c r="E68" s="1">
         <v>4</v>
@@ -2260,16 +2260,16 @@
         <v>98</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D69" s="4">
-        <v>43683.279046701391</v>
+        <v>43683.29877966435</v>
       </c>
       <c r="E69" s="1">
         <v>5</v>
       </c>
       <c r="F69" s="2">
-        <v>3.5113726851851851E-2</v>
+        <v>5.8349479166666662E-2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,16 +2280,16 @@
         <v>98</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70" s="4">
-        <v>43683.328310555553</v>
+        <v>43683.329030636574</v>
       </c>
       <c r="E70" s="1">
         <v>2</v>
       </c>
       <c r="F70" s="2">
-        <v>4.9263865740740743E-2</v>
+        <v>3.2096851851851856E-2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,16 +2300,16 @@
         <v>98</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D71" s="4">
-        <v>43683.339755717592</v>
+        <v>43683.365954259258</v>
       </c>
       <c r="E71" s="1">
         <v>4</v>
       </c>
       <c r="F71" s="2">
-        <v>1.1445162037037037E-2</v>
+        <v>3.0250972222222224E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2320,16 +2320,16 @@
         <v>98</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72" s="4">
-        <v>43683.373314155091</v>
+        <v>43683.385667511575</v>
       </c>
       <c r="E72" s="1">
         <v>4</v>
       </c>
       <c r="F72" s="2">
-        <v>3.3558437500000003E-2</v>
+        <v>3.6923622685185183E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2340,16 +2340,16 @@
         <v>98</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D73" s="4">
-        <v>43683.405390497683</v>
+        <v>43683.408954247687</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
       </c>
       <c r="F73" s="2">
-        <v>3.2076342592592594E-2</v>
+        <v>1.9713252314814814E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2360,10 +2360,10 @@
         <v>102</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" s="4">
-        <v>43683.244171319442</v>
+        <v>43683.251941620372</v>
       </c>
       <c r="E74" s="1">
         <v>2</v>
@@ -2378,7 +2378,7 @@
         <v>102</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D75" s="4">
         <v>43683.271920833336</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="2">
-        <v>2.7749502314814812E-2</v>
+        <v>4.3608287037037036E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2398,16 +2398,16 @@
         <v>102</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D76" s="4">
-        <v>43683.283804398146</v>
+        <v>43683.367624050923</v>
       </c>
       <c r="E76" s="1">
         <v>17</v>
       </c>
       <c r="F76" s="2">
-        <v>1.1883564814814814E-2</v>
+        <v>1.9979212962962963E-2</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,10 +2418,10 @@
         <v>103</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D77" s="4">
-        <v>43683.22648099537</v>
+        <v>43683.251959085646</v>
       </c>
       <c r="E77" s="1">
         <v>6</v>
@@ -2436,16 +2436,16 @@
         <v>103</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D78" s="4">
-        <v>43683.318651770831</v>
+        <v>43683.324824930554</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
       </c>
       <c r="F78" s="2">
-        <v>9.2170763888888896E-2</v>
+        <v>4.362575231481481E-2</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,16 +2456,16 @@
         <v>103</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D79" s="4">
-        <v>43683.349221863427</v>
+        <v>43683.384297048608</v>
       </c>
       <c r="E79" s="1">
         <v>9</v>
       </c>
       <c r="F79" s="2">
-        <v>3.0570104166666667E-2</v>
+        <v>7.2865844907407398E-2</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2476,16 +2476,16 @@
         <v>103</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D80" s="4">
-        <v>43683.393102187503</v>
+        <v>43683.411429282409</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
       </c>
       <c r="F80" s="2">
-        <v>4.3880324074074079E-2</v>
+        <v>5.9472118055555558E-2</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
         <v>105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D81" s="4">
         <v>43683.248300196756</v>
@@ -2514,16 +2514,16 @@
         <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D82" s="4">
-        <v>43683.307250879632</v>
+        <v>43683.323808252317</v>
       </c>
       <c r="E82" s="1">
         <v>4</v>
       </c>
       <c r="F82" s="2">
-        <v>5.895068287037037E-2</v>
+        <v>3.9966863425925932E-2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2534,16 +2534,16 @@
         <v>105</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D83" s="4">
-        <v>43683.343602037035</v>
+        <v>43683.410861087963</v>
       </c>
       <c r="E83" s="1">
         <v>4</v>
       </c>
       <c r="F83" s="2">
-        <v>3.6351157407407408E-2</v>
+        <v>7.550805555555555E-2</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2554,10 +2554,10 @@
         <v>106</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" s="4">
-        <v>43683.216844490744</v>
+        <v>43683.228506122687</v>
       </c>
       <c r="E84" s="1">
         <v>3</v>
@@ -2572,16 +2572,16 @@
         <v>106</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D85" s="4">
-        <v>43683.249709571763</v>
+        <v>43683.251915011577</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
       </c>
       <c r="F85" s="2">
-        <v>3.2865069444444443E-2</v>
+        <v>2.0172789351851853E-2</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2592,16 +2592,16 @@
         <v>106</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D86" s="4">
-        <v>43683.268378009256</v>
+        <v>43683.30471207176</v>
       </c>
       <c r="E86" s="1">
         <v>6</v>
       </c>
       <c r="F86" s="2">
-        <v>1.8668437499999999E-2</v>
+        <v>2.3408888888888885E-2</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,16 +2612,16 @@
         <v>106</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D87" s="4">
-        <v>43683.314402881944</v>
+        <v>43683.371969525462</v>
       </c>
       <c r="E87" s="1">
         <v>12</v>
       </c>
       <c r="F87" s="2">
-        <v>4.6024872685185181E-2</v>
+        <v>5.2797060185185186E-2</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
         <v>106</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D88" s="4">
         <v>43683.389847662038</v>
@@ -2641,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="2">
-        <v>7.5444780092592589E-2</v>
+        <v>6.7257453703703701E-2</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2652,10 +2652,10 @@
         <v>107</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D89" s="4">
-        <v>43683.21717650463</v>
+        <v>43683.226555138892</v>
       </c>
       <c r="E89" s="1">
         <v>3</v>
@@ -2670,16 +2670,16 @@
         <v>107</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" s="4">
-        <v>43683.269379131947</v>
+        <v>43683.285867650462</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
       </c>
       <c r="F90" s="2">
-        <v>5.2202638888888896E-2</v>
+        <v>1.8221805555555557E-2</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2690,16 +2690,16 @@
         <v>107</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D91" s="4">
-        <v>43683.316187511577</v>
+        <v>43683.413797372683</v>
       </c>
       <c r="E91" s="1">
         <v>17</v>
       </c>
       <c r="F91" s="2">
-        <v>4.680837962962963E-2</v>
+        <v>5.9312511574074078E-2</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2710,10 +2710,10 @@
         <v>108</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D92" s="4">
-        <v>43683.225241886576</v>
+        <v>43683.234231643517</v>
       </c>
       <c r="E92" s="1">
         <v>2</v>
@@ -2728,16 +2728,16 @@
         <v>108</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D93" s="4">
-        <v>43683.287758935185</v>
+        <v>43683.298521770834</v>
       </c>
       <c r="E93" s="1">
         <v>3</v>
       </c>
       <c r="F93" s="2">
-        <v>6.2517048611111112E-2</v>
+        <v>2.5898310185185184E-2</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2748,16 +2748,16 @@
         <v>108</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" s="4">
-        <v>43683.332332847225</v>
+        <v>43683.41422677083</v>
       </c>
       <c r="E94" s="1">
         <v>8</v>
       </c>
       <c r="F94" s="2">
-        <v>4.4573912037037033E-2</v>
+        <v>6.4290127314814816E-2</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2768,10 +2768,10 @@
         <v>110</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D95" s="4">
-        <v>43683.215547222222</v>
+        <v>43683.226243761572</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -2786,16 +2786,16 @@
         <v>110</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D96" s="4">
-        <v>43683.252002893518</v>
+        <v>43683.257642627315</v>
       </c>
       <c r="E96" s="1">
         <v>3</v>
       </c>
       <c r="F96" s="2">
-        <v>3.6455671296296295E-2</v>
+        <v>1.7910428240740742E-2</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2806,16 +2806,16 @@
         <v>110</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D97" s="4">
-        <v>43683.26969079861</v>
+        <v>43683.278019166668</v>
       </c>
       <c r="E97" s="1">
         <v>2</v>
       </c>
       <c r="F97" s="2">
-        <v>1.7687905092592594E-2</v>
+        <v>3.1398877314814812E-2</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2826,16 +2826,16 @@
         <v>110</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D98" s="4">
-        <v>43683.287677534725</v>
+        <v>43683.288635266203</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
       </c>
       <c r="F98" s="2">
-        <v>1.7986747685185187E-2</v>
+        <v>2.0376539351851849E-2</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2846,16 +2846,16 @@
         <v>110</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D99" s="4">
-        <v>43683.296595856482</v>
+        <v>43683.298159791666</v>
       </c>
       <c r="E99" s="1">
         <v>2</v>
       </c>
       <c r="F99" s="2">
-        <v>8.9183217592592595E-3</v>
+        <v>1.0616099537037037E-2</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2866,16 +2866,16 @@
         <v>110</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D100" s="4">
-        <v>43683.319476886572</v>
+        <v>43683.410022013886</v>
       </c>
       <c r="E100" s="1">
         <v>6</v>
       </c>
       <c r="F100" s="2">
-        <v>2.2881030092592593E-2</v>
+        <v>9.5245254629629638E-3</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2886,10 +2886,10 @@
         <v>111</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D101" s="4">
-        <v>43683.216709895831</v>
+        <v>43683.231319108796</v>
       </c>
       <c r="E101" s="1">
         <v>3</v>
@@ -2904,16 +2904,16 @@
         <v>111</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D102" s="4">
-        <v>43683.276819039354</v>
+        <v>43683.299067361113</v>
       </c>
       <c r="E102" s="1">
         <v>3</v>
       </c>
       <c r="F102" s="2">
-        <v>6.0109143518518517E-2</v>
+        <v>2.2985775462962963E-2</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2924,16 +2924,16 @@
         <v>111</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D103" s="4">
-        <v>43683.314152708335</v>
+        <v>43683.32012434028</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
       </c>
       <c r="F103" s="2">
-        <v>3.733366898148148E-2</v>
+        <v>6.7748252314814808E-2</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2944,16 +2944,16 @@
         <v>111</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D104" s="4">
-        <v>43683.380014861112</v>
+        <v>43683.41243449074</v>
       </c>
       <c r="E104" s="1">
         <v>4</v>
       </c>
       <c r="F104" s="2">
-        <v>6.586215277777778E-2</v>
+        <v>2.1056979166666667E-2</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>134</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D105" s="4">
         <v>43683.257551875002</v>
@@ -2982,16 +2982,16 @@
         <v>134</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106" s="4">
-        <v>43683.27176520833</v>
+        <v>43683.274935046298</v>
       </c>
       <c r="E106" s="1">
         <v>2</v>
       </c>
       <c r="F106" s="2">
-        <v>1.4213344907407407E-2</v>
+        <v>4.9218541666666671E-2</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3002,16 +3002,16 @@
         <v>134</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D107" s="4">
-        <v>43683.280269618059</v>
+        <v>43683.292000995367</v>
       </c>
       <c r="E107" s="1">
         <v>2</v>
       </c>
       <c r="F107" s="2">
-        <v>8.5044097222222222E-3</v>
+        <v>1.7383171296296296E-2</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,16 +3022,16 @@
         <v>134</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D108" s="4">
-        <v>43683.302108368058</v>
+        <v>43683.302889895836</v>
       </c>
       <c r="E108" s="1">
         <v>2</v>
       </c>
       <c r="F108" s="2">
-        <v>2.1838738425925926E-2</v>
+        <v>1.7065949074074074E-2</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,16 +3042,16 @@
         <v>134</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D109" s="4">
-        <v>43683.329894548609</v>
+        <v>43683.356877013888</v>
       </c>
       <c r="E109" s="1">
         <v>5</v>
       </c>
       <c r="F109" s="2">
-        <v>2.7786180555555554E-2</v>
+        <v>1.0888900462962965E-2</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,16 +3062,16 @@
         <v>134</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D110" s="4">
-        <v>43683.362301122688</v>
+        <v>43683.373660532408</v>
       </c>
       <c r="E110" s="1">
         <v>8</v>
       </c>
       <c r="F110" s="2">
-        <v>3.2406574074074074E-2</v>
+        <v>5.3987118055555561E-2</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
         <v>138</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D111" s="4">
         <v>43683.219107870369</v>
@@ -3100,7 +3100,7 @@
         <v>138</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D112" s="4">
         <v>43683.258474363429</v>
@@ -3109,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="F112" s="2">
-        <v>3.9366493055555556E-2</v>
+        <v>1.0774537037037036E-2</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,16 +3120,16 @@
         <v>138</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D113" s="4">
-        <v>43683.278884270832</v>
+        <v>43683.280053101851</v>
       </c>
       <c r="E113" s="1">
         <v>2</v>
       </c>
       <c r="F113" s="2">
-        <v>2.0409907407407408E-2</v>
+        <v>3.9366493055555556E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3140,16 +3140,16 @@
         <v>138</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D114" s="4">
-        <v>43683.294039872686</v>
+        <v>43683.356521782407</v>
       </c>
       <c r="E114" s="1">
         <v>19</v>
       </c>
       <c r="F114" s="2">
-        <v>1.5155601851851852E-2</v>
+        <v>2.1578738425925923E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3160,16 +3160,16 @@
         <v>138</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D115" s="4">
-        <v>43683.370746562498</v>
+        <v>43683.415673391202</v>
       </c>
       <c r="E115" s="1">
         <v>15</v>
       </c>
       <c r="F115" s="2">
-        <v>7.6706689814814821E-2</v>
+        <v>7.6468680555555557E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3180,10 +3180,10 @@
         <v>158</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D116" s="4">
-        <v>43683.262251701388</v>
+        <v>43683.28129997685</v>
       </c>
       <c r="E116" s="1">
         <v>4</v>
@@ -3198,16 +3198,16 @@
         <v>158</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D117" s="4">
-        <v>43683.300732025462</v>
+        <v>43683.3161740625</v>
       </c>
       <c r="E117" s="1">
         <v>2</v>
       </c>
       <c r="F117" s="2">
-        <v>3.8480324074074077E-2</v>
+        <v>7.2966643518518517E-2</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>158</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D118" s="4">
         <v>43683.348097268521</v>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="F118" s="2">
-        <v>4.736523148148148E-2</v>
+        <v>3.4874085648148145E-2</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3238,16 +3238,16 @@
         <v>158</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D119" s="4">
-        <v>43683.391411458331</v>
+        <v>43683.408193460651</v>
       </c>
       <c r="E119" s="1">
         <v>3</v>
       </c>
       <c r="F119" s="2">
-        <v>4.331420138888889E-2</v>
+        <v>3.1923206018518523E-2</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3258,16 +3258,16 @@
         <v>158</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D120" s="4">
-        <v>43683.40827659722</v>
+        <v>43683.415212476852</v>
       </c>
       <c r="E120" s="1">
         <v>3</v>
       </c>
       <c r="F120" s="2">
-        <v>1.6865138888888888E-2</v>
+        <v>6.0096192129629633E-2</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3278,10 +3278,10 @@
         <v>174</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D121" s="4">
-        <v>43683.266281365744</v>
+        <v>43683.282273935183</v>
       </c>
       <c r="E121" s="1">
         <v>7</v>
@@ -3296,7 +3296,7 @@
         <v>174</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D122" s="4">
         <v>43683.301574965277</v>
@@ -3305,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="2">
-        <v>3.5293611111111116E-2</v>
+        <v>7.3940601851851848E-2</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3316,16 +3316,16 @@
         <v>174</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D123" s="4">
-        <v>43683.305733518515</v>
+        <v>43683.318776817126</v>
       </c>
       <c r="E123" s="1">
         <v>5</v>
       </c>
       <c r="F123" s="2">
-        <v>4.1585416666666663E-3</v>
+        <v>1.9301030092592594E-2</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3336,16 +3336,16 @@
         <v>174</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D124" s="4">
-        <v>43683.355091076388</v>
+        <v>43683.359789513888</v>
       </c>
       <c r="E124" s="1">
         <v>3</v>
       </c>
       <c r="F124" s="2">
-        <v>4.9357569444444443E-2</v>
+        <v>1.7201840277777779E-2</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3356,16 +3356,16 @@
         <v>174</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D125" s="4">
-        <v>43683.363719456021</v>
+        <v>43683.390629988426</v>
       </c>
       <c r="E125" s="1">
         <v>3</v>
       </c>
       <c r="F125" s="2">
-        <v>8.6283680555555558E-3</v>
+        <v>4.1012708333333335E-2</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3376,16 +3376,16 @@
         <v>174</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D126" s="4">
-        <v>43683.396443090278</v>
+        <v>43683.397608252315</v>
       </c>
       <c r="E126" s="1">
         <v>2</v>
       </c>
       <c r="F126" s="2">
-        <v>3.2723634259259261E-2</v>
+        <v>3.0840474537037036E-2</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3396,10 +3396,10 @@
         <v>194</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D127" s="4">
-        <v>43683.254015243052</v>
+        <v>43683.265935740739</v>
       </c>
       <c r="E127" s="1">
         <v>5</v>
@@ -3414,16 +3414,16 @@
         <v>194</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D128" s="4">
-        <v>43683.272544733794</v>
+        <v>43683.311824502314</v>
       </c>
       <c r="E128" s="1">
         <v>6</v>
       </c>
       <c r="F128" s="2">
-        <v>1.8529479166666665E-2</v>
+        <v>5.7602407407407408E-2</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3434,16 +3434,16 @@
         <v>194</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D129" s="4">
-        <v>43683.318468206016</v>
+        <v>43683.326047314818</v>
       </c>
       <c r="E129" s="1">
         <v>2</v>
       </c>
       <c r="F129" s="2">
-        <v>4.5923483796296294E-2</v>
+        <v>4.5888761574074073E-2</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -3454,16 +3454,16 @@
         <v>194</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D130" s="4">
-        <v>43683.339190601851</v>
+        <v>43683.385075787039</v>
       </c>
       <c r="E130" s="1">
         <v>19</v>
       </c>
       <c r="F130" s="2">
-        <v>2.0722395833333334E-2</v>
+        <v>1.4222812500000001E-2</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -3474,16 +3474,16 @@
         <v>194</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D131" s="4">
-        <v>43683.388752395833</v>
+        <v>43683.41371601852</v>
       </c>
       <c r="E131" s="1">
         <v>12</v>
       </c>
       <c r="F131" s="2">
-        <v>4.9561793981481479E-2</v>
+        <v>5.9028483796296292E-2</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,16 +3494,16 @@
         <v>194</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D132" s="4">
-        <v>43683.413850474535</v>
+        <v>43683.41415571759</v>
       </c>
       <c r="E132" s="1">
         <v>3</v>
       </c>
       <c r="F132" s="2">
-        <v>2.5098078703703702E-2</v>
+        <v>2.8640231481481482E-2</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -3514,10 +3514,10 @@
         <v>197</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D133" s="4">
-        <v>43683.26959009259</v>
+        <v>43683.27241553241</v>
       </c>
       <c r="E133" s="1">
         <v>2</v>
@@ -3532,16 +3532,16 @@
         <v>197</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D134" s="4">
-        <v>43683.296019236113</v>
+        <v>43683.334198460645</v>
       </c>
       <c r="E134" s="1">
         <v>7</v>
       </c>
       <c r="F134" s="2">
-        <v>2.6429143518518518E-2</v>
+        <v>6.4082199074074073E-2</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -3552,16 +3552,16 @@
         <v>197</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D135" s="4">
-        <v>43683.351719548613</v>
+        <v>43683.360342175925</v>
       </c>
       <c r="E135" s="1">
         <v>4</v>
       </c>
       <c r="F135" s="2">
-        <v>5.5700312499999995E-2</v>
+        <v>6.1782939814814815E-2</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>197</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D136" s="4">
         <v>43683.382490775461</v>
@@ -3581,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="F136" s="2">
-        <v>3.0771238425925926E-2</v>
+        <v>2.6143715277777774E-2</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3592,16 +3592,16 @@
         <v>197</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D137" s="4">
-        <v>43683.390765138887</v>
+        <v>43683.415288368058</v>
       </c>
       <c r="E137" s="1">
         <v>3</v>
       </c>
       <c r="F137" s="2">
-        <v>8.2743518518518504E-3</v>
+        <v>2.2148599537037041E-2</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3612,10 +3612,10 @@
         <v>214</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D138" s="4">
-        <v>43683.22127011574</v>
+        <v>43683.239178750002</v>
       </c>
       <c r="E138" s="1">
         <v>2</v>
@@ -3630,16 +3630,16 @@
         <v>214</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D139" s="4">
-        <v>43683.279857013891</v>
+        <v>43683.301000844906</v>
       </c>
       <c r="E139" s="1">
         <v>4</v>
       </c>
       <c r="F139" s="2">
-        <v>5.8586898148148152E-2</v>
+        <v>3.0845416666666667E-2</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3650,7 +3650,7 @@
         <v>214</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D140" s="4">
         <v>43683.313017708337</v>
@@ -3659,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="F140" s="2">
-        <v>3.3160694444444444E-2</v>
+        <v>6.18220949074074E-2</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3670,7 +3670,7 @@
         <v>214</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D141" s="4">
         <v>43683.321579976851</v>
@@ -3679,7 +3679,7 @@
         <v>1</v>
       </c>
       <c r="F141" s="2">
-        <v>8.5622685185185194E-3</v>
+        <v>1.2016863425925927E-2</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -3690,16 +3690,16 @@
         <v>214</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D142" s="4">
-        <v>43683.326384745371</v>
+        <v>43683.413990949077</v>
       </c>
       <c r="E142" s="1">
         <v>34</v>
       </c>
       <c r="F142" s="2">
-        <v>4.8047685185185181E-3</v>
+        <v>8.5622685185185194E-3</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3710,10 +3710,10 @@
         <v>250</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D143" s="4">
-        <v>43683.217182685185</v>
+        <v>43683.239056759259</v>
       </c>
       <c r="E143" s="1">
         <v>5</v>
@@ -3728,16 +3728,16 @@
         <v>250</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D144" s="4">
-        <v>43683.253050196756</v>
+        <v>43683.274063391204</v>
       </c>
       <c r="E144" s="1">
         <v>8</v>
       </c>
       <c r="F144" s="2">
-        <v>3.5867523148148152E-2</v>
+        <v>3.0723425925925928E-2</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3748,16 +3748,16 @@
         <v>250</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D145" s="4">
-        <v>43683.29973013889</v>
+        <v>43683.312795659724</v>
       </c>
       <c r="E145" s="1">
         <v>5</v>
       </c>
       <c r="F145" s="2">
-        <v>4.6679930555555554E-2</v>
+        <v>3.5006631944444443E-2</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3768,16 +3768,16 @@
         <v>250</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D146" s="4">
-        <v>43683.316533935184</v>
+        <v>43683.355712280092</v>
       </c>
       <c r="E146" s="1">
         <v>13</v>
       </c>
       <c r="F146" s="2">
-        <v>1.680380787037037E-2</v>
+        <v>3.873226851851852E-2</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3788,16 +3788,16 @@
         <v>250</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D147" s="4">
-        <v>43683.367566261571</v>
+        <v>43683.415486493053</v>
       </c>
       <c r="E147" s="1">
         <v>27</v>
       </c>
       <c r="F147" s="2">
-        <v>5.1032314814814815E-2</v>
+        <v>4.2916620370370369E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update i3 script and excel to include 0 time
</commit_message>
<xml_diff>
--- a/insights/3/solution_approaches.xlsx
+++ b/insights/3/solution_approaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\insights\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852052ED-BED5-4813-A9F9-822BFAF68A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5DF723-B8EA-418B-9566-3C83F62ACD3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +952,9 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1090,7 +1092,9 @@
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1228,7 +1232,9 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1386,7 +1392,9 @@
       <c r="E24" s="1">
         <v>8</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1444,7 +1452,9 @@
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1602,7 +1612,9 @@
       <c r="E35" s="1">
         <v>5</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1700,7 +1712,9 @@
       <c r="E40" s="1">
         <v>1</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -1858,7 +1872,9 @@
       <c r="E48" s="1">
         <v>8</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -1936,7 +1952,9 @@
       <c r="E52" s="1">
         <v>2</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -2034,7 +2052,9 @@
       <c r="E57" s="1">
         <v>11</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
@@ -2152,7 +2172,9 @@
       <c r="E63" s="1">
         <v>10</v>
       </c>
-      <c r="F63" s="2"/>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -2250,7 +2272,9 @@
       <c r="E68" s="1">
         <v>4</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -2368,7 +2392,9 @@
       <c r="E74" s="1">
         <v>2</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -2426,7 +2452,9 @@
       <c r="E77" s="1">
         <v>6</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -2504,7 +2532,9 @@
       <c r="E81" s="1">
         <v>1</v>
       </c>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -2562,7 +2592,9 @@
       <c r="E84" s="1">
         <v>3</v>
       </c>
-      <c r="F84" s="2"/>
+      <c r="F84" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
@@ -2660,7 +2692,9 @@
       <c r="E89" s="1">
         <v>3</v>
       </c>
-      <c r="F89" s="2"/>
+      <c r="F89" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -2718,7 +2752,9 @@
       <c r="E92" s="1">
         <v>2</v>
       </c>
-      <c r="F92" s="2"/>
+      <c r="F92" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
@@ -2776,7 +2812,9 @@
       <c r="E95" s="1">
         <v>3</v>
       </c>
-      <c r="F95" s="2"/>
+      <c r="F95" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
@@ -2894,7 +2932,9 @@
       <c r="E101" s="1">
         <v>3</v>
       </c>
-      <c r="F101" s="2"/>
+      <c r="F101" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
@@ -2972,7 +3012,9 @@
       <c r="E105" s="1">
         <v>1</v>
       </c>
-      <c r="F105" s="2"/>
+      <c r="F105" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -3090,7 +3132,9 @@
       <c r="E111" s="1">
         <v>1</v>
       </c>
-      <c r="F111" s="2"/>
+      <c r="F111" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
@@ -3188,7 +3232,9 @@
       <c r="E116" s="1">
         <v>4</v>
       </c>
-      <c r="F116" s="2"/>
+      <c r="F116" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
@@ -3286,7 +3332,9 @@
       <c r="E121" s="1">
         <v>7</v>
       </c>
-      <c r="F121" s="2"/>
+      <c r="F121" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -3404,7 +3452,9 @@
       <c r="E127" s="1">
         <v>5</v>
       </c>
-      <c r="F127" s="2"/>
+      <c r="F127" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
@@ -3522,7 +3572,9 @@
       <c r="E133" s="1">
         <v>2</v>
       </c>
-      <c r="F133" s="2"/>
+      <c r="F133" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
@@ -3620,7 +3672,9 @@
       <c r="E138" s="1">
         <v>2</v>
       </c>
-      <c r="F138" s="2"/>
+      <c r="F138" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
@@ -3718,7 +3772,9 @@
       <c r="E143" s="1">
         <v>5</v>
       </c>
-      <c r="F143" s="2"/>
+      <c r="F143" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">

</xml_diff>